<commit_message>
Updated BLK, ULTA, LVMH models
</commit_message>
<xml_diff>
--- a/Still Researching/FTNT.xlsx
+++ b/Still Researching/FTNT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bina/Documents/financial-modeling/Still Researching/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77397A44-7CFC-D147-A03D-BAE9E6315B45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00BD33DF-D2E2-C64D-A5A6-F8FB6B8ABB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -2120,16 +2120,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>21166</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>222954</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>35275</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>25398</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>28223</xdr:colOff>
-      <xdr:row>62</xdr:row>
-      <xdr:rowOff>42333</xdr:rowOff>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>1608666</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2456,11 +2456,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL118"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="I84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
+      <selection pane="bottomRight" activeCell="P123" sqref="P123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>